<commit_message>
New Excel table of products
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{8A3AE7B2-930A-413D-9CD5-E12AA5FA2613}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F2B92CD6-CA45-4836-8F28-B7D819ED1B0F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="121">
   <si>
     <t>Id</t>
   </si>
@@ -158,6 +158,231 @@
   </si>
   <si>
     <t>קומקום תה יפיפה עיטור בורדו , נוף הולנדי</t>
+  </si>
+  <si>
+    <t>סטנד לביצים</t>
+  </si>
+  <si>
+    <t>עץ</t>
+  </si>
+  <si>
+    <t>מנדולינה (חותך כרוב)</t>
+  </si>
+  <si>
+    <t>קרש חיתוך ענק</t>
+  </si>
+  <si>
+    <t>קרש חיתוך ישן</t>
+  </si>
+  <si>
+    <t>קרש חיתוך עתיק</t>
+  </si>
+  <si>
+    <t>מלחיה בצורת חבית לתלייה</t>
+  </si>
+  <si>
+    <t>מלחיה גדולה בצורת חבית לתלייה</t>
+  </si>
+  <si>
+    <t>מלחייה לתלייה</t>
+  </si>
+  <si>
+    <t>מכתש ועלי גדול</t>
+  </si>
+  <si>
+    <t>מכתש ועלי קטן</t>
+  </si>
+  <si>
+    <t>קופסה אליפטית</t>
+  </si>
+  <si>
+    <t>קופסה אליפטית, עץ דק</t>
+  </si>
+  <si>
+    <t>חותך כרוב ענק (מנדולינה)</t>
+  </si>
+  <si>
+    <t>קופסה לתלייה</t>
+  </si>
+  <si>
+    <t>מטחנת קפה צרפתית , Peugeot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">מטחנת קפה הולנדית PE-DE </t>
+  </si>
+  <si>
+    <t>ארגז סכו"ם יפיפה</t>
+  </si>
+  <si>
+    <t>מגש עם דפנות גבוהות</t>
+  </si>
+  <si>
+    <t>ארגז לסכו"ם</t>
+  </si>
+  <si>
+    <t xml:space="preserve">סל עץ עם ידית מתכת </t>
+  </si>
+  <si>
+    <t>סל עץ גדול</t>
+  </si>
+  <si>
+    <t>קופסה רב שימושית</t>
+  </si>
+  <si>
+    <t>פומפיה גדולה</t>
+  </si>
+  <si>
+    <t>מתכת</t>
+  </si>
+  <si>
+    <t>פח</t>
+  </si>
+  <si>
+    <t>פומפיה 3 צלעות מיוחדת חומר מתכתי</t>
+  </si>
+  <si>
+    <t xml:space="preserve">פומפיה 3 צלעות מיוחדת </t>
+  </si>
+  <si>
+    <t>פומפיה מרובעת</t>
+  </si>
+  <si>
+    <t>פומפיה גליל</t>
+  </si>
+  <si>
+    <t>פומפיה ענקית</t>
+  </si>
+  <si>
+    <t>תבנית עוגה</t>
+  </si>
+  <si>
+    <t>תבנית אליפטית גדולה</t>
+  </si>
+  <si>
+    <t>תבנית קטנה</t>
+  </si>
+  <si>
+    <t>תבנית עוגות מדלן</t>
+  </si>
+  <si>
+    <t>תבנית שוקלד - מתכת</t>
+  </si>
+  <si>
+    <t>תבנית עוגות אישיות - מתכת</t>
+  </si>
+  <si>
+    <t>סל ביצים - חוט מתכת</t>
+  </si>
+  <si>
+    <t>סל ביצים , חוט מתכת</t>
+  </si>
+  <si>
+    <t>סל ביצים מיוחד מתקפל</t>
+  </si>
+  <si>
+    <t>סל בקבוקים , מתכת</t>
+  </si>
+  <si>
+    <t>קופסה שאבי שיק</t>
+  </si>
+  <si>
+    <t>ארגז גדול הולנדי , שאבי שיק</t>
+  </si>
+  <si>
+    <t>ארגז גדול הולנדי (שאבי שוק)</t>
+  </si>
+  <si>
+    <t>קופסת עוגיות עם חלון זכוכית</t>
+  </si>
+  <si>
+    <t>מגש ציור יד , המאה ה-19 , צרפת</t>
+  </si>
+  <si>
+    <t>זוג קפסאות איכסון הולנדיות</t>
+  </si>
+  <si>
+    <t>פעמון לכיסוי אוכל המאה ה-19 ארט-נובו</t>
+  </si>
+  <si>
+    <t>פעמון לכיסוי אוכל המאה ה-19</t>
+  </si>
+  <si>
+    <t>פינטר</t>
+  </si>
+  <si>
+    <t>Sub-Category</t>
+  </si>
+  <si>
+    <t>דקורציה</t>
+  </si>
+  <si>
+    <t>ארגז</t>
+  </si>
+  <si>
+    <t>מגש</t>
+  </si>
+  <si>
+    <t>מטבח</t>
+  </si>
+  <si>
+    <t>קופסה</t>
+  </si>
+  <si>
+    <t>כד</t>
+  </si>
+  <si>
+    <t>קומקום</t>
+  </si>
+  <si>
+    <t>מלחייה</t>
+  </si>
+  <si>
+    <t>איחסון</t>
+  </si>
+  <si>
+    <t>פמוט</t>
+  </si>
+  <si>
+    <t>נדרש תמונה</t>
+  </si>
+  <si>
+    <t>צלחת הגשה</t>
+  </si>
+  <si>
+    <t>סט קפה</t>
+  </si>
+  <si>
+    <t>מגש גבינות</t>
+  </si>
+  <si>
+    <t>כלי עבודה</t>
+  </si>
+  <si>
+    <t>מטחנה</t>
+  </si>
+  <si>
+    <t>סל</t>
+  </si>
+  <si>
+    <t>פומפיה</t>
+  </si>
+  <si>
+    <t>תבנית עוגה מקסימה</t>
+  </si>
+  <si>
+    <t>תבנית</t>
+  </si>
+  <si>
+    <t>תבנית עוגה קטנה</t>
+  </si>
+  <si>
+    <t>תבנית עוגיות מדלן</t>
+  </si>
+  <si>
+    <t>סל ביצים פתוח, חוט מתכת</t>
+  </si>
+  <si>
+    <t>הגשה</t>
   </si>
 </sst>
 </file>
@@ -208,10 +433,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,19 +721,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2417CC-E9D4-4575-BBAA-5E76F42A36C1}">
-  <dimension ref="B2:K33"/>
+  <dimension ref="A2:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="F70" sqref="F70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="9.75" customWidth="1"/>
-    <col min="10" max="11" width="21.9140625" customWidth="1"/>
+    <col min="11" max="12" width="21.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,25 +747,28 @@
         <v>3</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -550,26 +781,29 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="1">
         <v>26.5</v>
       </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="1">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>420</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="84" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="84" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -582,26 +816,29 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="1">
         <v>28</v>
       </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="98" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="98" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -614,26 +851,29 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="1">
         <v>15.5</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>36.5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>12.5</v>
       </c>
-      <c r="I5" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="56" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -646,26 +886,29 @@
       <c r="E6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" s="1">
         <v>22</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>15</v>
       </c>
-      <c r="H6" s="1">
-        <v>11</v>
-      </c>
-      <c r="I6" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6" s="1">
+        <v>11</v>
+      </c>
+      <c r="J6" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="98" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="98" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -678,26 +921,29 @@
       <c r="E7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G7" s="1">
         <v>26</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
       <c r="H7" s="1">
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -708,28 +954,31 @@
         <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
+        <v>97</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>106</v>
       </c>
       <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
         <v>17.5</v>
       </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="1">
+      <c r="L8" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="112" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="112" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -742,26 +991,29 @@
       <c r="E9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="1">
         <v>19</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>13</v>
       </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="1">
+      <c r="L9" s="1">
         <v>850</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -774,26 +1026,32 @@
       <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="1">
         <v>26</v>
       </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
       <c r="H10" s="1">
         <v>0</v>
       </c>
-      <c r="I10" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1" t="s">
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>107</v>
+      </c>
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -806,26 +1064,29 @@
       <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="1">
         <v>38.5</v>
       </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
       <c r="H11" s="1">
         <v>0</v>
       </c>
-      <c r="I11" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1" t="s">
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="1">
+      <c r="L11" s="1">
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="84" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="84" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -838,26 +1099,29 @@
       <c r="E12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G12" s="1">
         <v>16.5</v>
       </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
       <c r="H12" s="1">
         <v>0</v>
       </c>
-      <c r="I12" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1" t="s">
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -870,26 +1134,29 @@
       <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="1">
         <v>21</v>
       </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
       <c r="H13" s="1">
         <v>0</v>
       </c>
-      <c r="I13" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1" t="s">
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="98" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="98" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -902,26 +1169,29 @@
       <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="1">
         <v>25</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>22.5</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>12</v>
       </c>
-      <c r="I14" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K14" s="1">
+      <c r="L14" s="1">
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="56" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="56" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -934,26 +1204,29 @@
       <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
+      <c r="F15" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G15" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <v>32</v>
       </c>
-      <c r="I15" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1" t="s">
+      <c r="I15" s="1">
+        <v>32</v>
+      </c>
+      <c r="J15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="1">
+      <c r="L15" s="1">
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -966,26 +1239,29 @@
       <c r="E16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="1">
-        <v>0</v>
+      <c r="F16" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G16" s="1">
-        <v>26.5</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
         <v>26.5</v>
       </c>
-      <c r="I16" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1" t="s">
+      <c r="I16" s="1">
+        <v>26.5</v>
+      </c>
+      <c r="J16" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K16" s="1">
+      <c r="L16" s="1">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -998,26 +1274,29 @@
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="1">
-        <v>0</v>
+      <c r="F17" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
         <v>24.5</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>32</v>
       </c>
-      <c r="I17" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="1">
+      <c r="L17" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1030,26 +1309,29 @@
       <c r="E18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="1">
         <v>13.5</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>24</v>
       </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1" t="s">
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1062,26 +1344,29 @@
       <c r="E19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G19" s="1">
         <v>7.5</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>14</v>
       </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1" t="s">
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>380</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -1094,8 +1379,8 @@
       <c r="E20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="1">
-        <v>0</v>
+      <c r="F20" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1103,17 +1388,20 @@
       <c r="H20" s="1">
         <v>0</v>
       </c>
-      <c r="I20" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="1" t="s">
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K20" s="1">
+      <c r="L20" s="1">
         <v>620</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="84" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="84" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1126,26 +1414,29 @@
       <c r="E21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="1">
-        <v>0</v>
+      <c r="F21" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G21" s="1">
-        <v>30.5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
         <v>30.5</v>
       </c>
-      <c r="I21" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="1" t="s">
+      <c r="I21" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="J21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="56" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="56" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -1158,26 +1449,29 @@
       <c r="E22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="1">
-        <v>0</v>
+      <c r="F22" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G22" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
         <v>32</v>
       </c>
-      <c r="I22" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="1" t="s">
+      <c r="I22" s="1">
+        <v>32</v>
+      </c>
+      <c r="J22" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K22" s="1">
+      <c r="L22" s="1">
         <v>270</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -1190,26 +1484,29 @@
       <c r="E23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="1">
-        <v>0</v>
+      <c r="F23" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="G23" s="1">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
         <v>33</v>
       </c>
-      <c r="I23" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="1" t="s">
+      <c r="I23" s="1">
+        <v>33</v>
+      </c>
+      <c r="J23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K23" s="1">
+      <c r="L23" s="1">
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="56" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="56" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -1222,8 +1519,8 @@
       <c r="E24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="1">
-        <v>0</v>
+      <c r="F24" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -1231,17 +1528,20 @@
       <c r="H24" s="1">
         <v>0</v>
       </c>
-      <c r="I24" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1" t="s">
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="K24" s="1">
+      <c r="L24" s="1">
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="112" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="112" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -1254,26 +1554,29 @@
       <c r="E25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F25" s="1">
-        <v>0</v>
+      <c r="F25" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
         <v>16</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>27</v>
       </c>
-      <c r="I25" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="1" t="s">
+      <c r="J25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K25" s="1">
+      <c r="L25" s="1">
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -1286,26 +1589,29 @@
       <c r="E26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="1">
         <v>20.5</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>12.5</v>
       </c>
-      <c r="H26" s="1">
-        <v>0</v>
-      </c>
-      <c r="I26" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" s="1" t="s">
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K26" s="1">
+      <c r="L26" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="70" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -1318,120 +1624,1532 @@
       <c r="E27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G27" s="1">
         <v>15</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>17</v>
       </c>
-      <c r="H27" s="1">
-        <v>0</v>
-      </c>
-      <c r="I27" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="1" t="s">
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K27" s="1">
+      <c r="L27" s="1">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>26</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G28" s="1">
+        <v>33</v>
+      </c>
+      <c r="H28" s="1">
+        <v>34</v>
+      </c>
+      <c r="I28" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="J28" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L28" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="42" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>27</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G29" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="H29" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L29" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>28</v>
       </c>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G30" s="1">
+        <v>42.5</v>
+      </c>
+      <c r="H30" s="1">
+        <v>29</v>
+      </c>
+      <c r="I30" s="1">
+        <v>6</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L30" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>29</v>
       </c>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G31" s="1">
+        <v>40</v>
+      </c>
+      <c r="H31" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I31" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="J31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="42" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>30</v>
       </c>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" s="1">
+        <v>44.5</v>
+      </c>
+      <c r="H32" s="1">
+        <v>20</v>
+      </c>
+      <c r="I32" s="1">
+        <v>3</v>
+      </c>
+      <c r="J32" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L32" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="56" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>31</v>
       </c>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G33" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="H33" s="1">
+        <v>16</v>
+      </c>
+      <c r="I33" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="J33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L33" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G34" s="1">
+        <v>25</v>
+      </c>
+      <c r="H34" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="I34" s="1">
+        <v>12</v>
+      </c>
+      <c r="J34" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L34" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="1">
+        <v>12</v>
+      </c>
+      <c r="H35" s="1">
+        <v>22</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0</v>
+      </c>
+      <c r="J35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L35" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="1">
+        <v>10</v>
+      </c>
+      <c r="H36" s="1">
+        <v>15</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0</v>
+      </c>
+      <c r="J36" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L36" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B37" s="1">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G37" s="1">
+        <v>21</v>
+      </c>
+      <c r="H37" s="1">
+        <v>30</v>
+      </c>
+      <c r="I37" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="J37" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L37" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B38" s="1">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="1">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1">
+        <v>23</v>
+      </c>
+      <c r="I38" s="1">
+        <v>64</v>
+      </c>
+      <c r="J38" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="L38" s="1">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="H39" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="I39" s="1">
+        <v>21</v>
+      </c>
+      <c r="J39" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L39" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G40" s="1">
+        <v>12</v>
+      </c>
+      <c r="H40" s="1">
+        <v>34</v>
+      </c>
+      <c r="I40" s="1">
+        <v>10.5</v>
+      </c>
+      <c r="J40" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+      <c r="B41" s="1">
+        <v>39</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G41" s="1">
+        <v>20</v>
+      </c>
+      <c r="H41" s="1">
+        <v>13</v>
+      </c>
+      <c r="I41" s="1">
+        <v>13</v>
+      </c>
+      <c r="J41" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L41" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+      <c r="B42" s="1">
+        <v>40</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" s="1">
+        <v>25</v>
+      </c>
+      <c r="H42" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="I42" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="J42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L42" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B43" s="1">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G43" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="H43" s="1">
+        <v>42</v>
+      </c>
+      <c r="I43" s="1">
+        <v>27</v>
+      </c>
+      <c r="J43" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L43" s="1">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B44" s="1">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" s="1">
+        <v>8</v>
+      </c>
+      <c r="H44" s="1">
+        <v>48</v>
+      </c>
+      <c r="I44" s="1">
+        <v>25</v>
+      </c>
+      <c r="J44" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L44" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B45" s="1">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="H45" s="1">
+        <v>41.5</v>
+      </c>
+      <c r="I45" s="1">
+        <v>29</v>
+      </c>
+      <c r="J45" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L45" s="1">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G46" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="H46" s="1">
+        <v>50</v>
+      </c>
+      <c r="I46" s="1">
+        <v>33.5</v>
+      </c>
+      <c r="J46" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L46" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B47" s="1">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="H47" s="1">
+        <v>39</v>
+      </c>
+      <c r="I47" s="1">
+        <v>28</v>
+      </c>
+      <c r="J47" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L47" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B48" s="1">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="I48" s="1">
+        <v>36</v>
+      </c>
+      <c r="J48" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L48" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B49" s="1">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G49" s="1">
+        <v>23</v>
+      </c>
+      <c r="H49" s="1">
+        <v>30</v>
+      </c>
+      <c r="I49" s="1">
+        <v>0</v>
+      </c>
+      <c r="J49" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L49" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>48</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G50" s="1">
+        <v>23</v>
+      </c>
+      <c r="H50" s="1">
+        <v>11</v>
+      </c>
+      <c r="I50" s="1">
+        <v>0</v>
+      </c>
+      <c r="J50" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L50" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B51" s="1">
+        <v>49</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G51" s="1">
+        <v>22</v>
+      </c>
+      <c r="H51" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="I51" s="1">
+        <v>0</v>
+      </c>
+      <c r="J51" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L51" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B52" s="1">
+        <v>50</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G52" s="1">
+        <v>48</v>
+      </c>
+      <c r="H52" s="1">
+        <v>21</v>
+      </c>
+      <c r="I52" s="1">
+        <v>0</v>
+      </c>
+      <c r="J52" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L52" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B53" s="1">
+        <v>51</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G53" s="1">
+        <v>13</v>
+      </c>
+      <c r="H53" s="1">
+        <v>16</v>
+      </c>
+      <c r="I53" s="1">
+        <v>0</v>
+      </c>
+      <c r="J53" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L53" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B54" s="1">
+        <v>52</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G54" s="1">
+        <v>12</v>
+      </c>
+      <c r="H54" s="1">
+        <v>15</v>
+      </c>
+      <c r="I54" s="1">
+        <v>0</v>
+      </c>
+      <c r="J54" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="L54" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B55" s="1">
+        <v>53</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G55" s="1">
+        <v>12</v>
+      </c>
+      <c r="H55" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="I55" s="1">
+        <v>17</v>
+      </c>
+      <c r="J55" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L55" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B56" s="1">
+        <v>54</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G56" s="1">
+        <v>8</v>
+      </c>
+      <c r="H56" s="1">
+        <v>17</v>
+      </c>
+      <c r="I56" s="1">
+        <v>0</v>
+      </c>
+      <c r="J56" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L56" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B57" s="1">
+        <v>55</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G57" s="1">
+        <v>7</v>
+      </c>
+      <c r="H57" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="I57" s="1">
+        <v>0</v>
+      </c>
+      <c r="J57" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L57" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B58" s="1">
+        <v>56</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>34</v>
+      </c>
+      <c r="I58" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="J58" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L58" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B59" s="1">
+        <v>57</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>28.5</v>
+      </c>
+      <c r="I59" s="1">
+        <v>14</v>
+      </c>
+      <c r="J59" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L59" s="1">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+      <c r="B60" s="1">
+        <v>58</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>27</v>
+      </c>
+      <c r="I60" s="1">
+        <v>26</v>
+      </c>
+      <c r="J60" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L60" s="1">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B61" s="1">
+        <v>59</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61" s="1">
+        <v>27</v>
+      </c>
+      <c r="H61" s="1">
+        <v>21</v>
+      </c>
+      <c r="I61" s="1">
+        <v>0</v>
+      </c>
+      <c r="J61" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L61" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B62" s="1">
+        <v>60</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G62" s="1">
+        <v>23</v>
+      </c>
+      <c r="H62" s="1">
+        <v>20</v>
+      </c>
+      <c r="I62" s="1">
+        <v>0</v>
+      </c>
+      <c r="J62" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L62" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B63" s="1">
+        <v>61</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G63" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="H63" s="1">
+        <v>34.5</v>
+      </c>
+      <c r="I63" s="1">
+        <v>0</v>
+      </c>
+      <c r="J63" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L63" s="1">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B64" s="1">
+        <v>62</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64" s="1">
+        <v>24</v>
+      </c>
+      <c r="H64" s="1">
+        <v>20</v>
+      </c>
+      <c r="I64" s="1">
+        <v>0</v>
+      </c>
+      <c r="J64" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L64" s="1">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+      <c r="B65" s="1">
+        <v>63</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G65" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="H65" s="1">
+        <v>24.5</v>
+      </c>
+      <c r="I65" s="1">
+        <v>20.5</v>
+      </c>
+      <c r="J65" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L65" s="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="66" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B66" s="1">
+        <v>64</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G66" s="1">
+        <v>25</v>
+      </c>
+      <c r="H66" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="I66" s="1">
+        <v>30</v>
+      </c>
+      <c r="J66" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L66" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="67" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="B67" s="1">
+        <v>65</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G67" s="1">
+        <v>10</v>
+      </c>
+      <c r="H67" s="1">
+        <v>23.5</v>
+      </c>
+      <c r="I67" s="1">
+        <v>22</v>
+      </c>
+      <c r="J67" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L67" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+      <c r="B68" s="1">
+        <v>66</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>40</v>
+      </c>
+      <c r="I68" s="1">
+        <v>0</v>
+      </c>
+      <c r="J68" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L68" s="1">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+      <c r="B69" s="1">
+        <v>67</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G69" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="H69" s="1">
+        <v>13</v>
+      </c>
+      <c r="I69" s="1">
+        <v>0</v>
+      </c>
+      <c r="J69" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L69" s="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+      <c r="B70" s="1">
+        <v>68</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G70" s="1">
+        <v>30</v>
+      </c>
+      <c r="H70" s="1">
+        <v>45</v>
+      </c>
+      <c r="I70" s="1">
+        <v>35</v>
+      </c>
+      <c r="J70" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L70" s="1">
+        <v>850</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
The finle .xlsx table.
</commit_message>
<xml_diff>
--- a/Products.xlsx
+++ b/Products.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{335D09A3-1734-456C-BF6D-6D3BED0C5DB6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{54CB3568-F856-4EB8-94CE-4917F22EC4BB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="135">
   <si>
     <t>Id</t>
   </si>
@@ -316,63 +316,18 @@
     <t>דקורציה</t>
   </si>
   <si>
-    <t>ארגז</t>
-  </si>
-  <si>
-    <t>מגש</t>
-  </si>
-  <si>
     <t>מטבח</t>
   </si>
   <si>
-    <t>קופסה</t>
-  </si>
-  <si>
-    <t>כד</t>
-  </si>
-  <si>
-    <t>קומקום</t>
-  </si>
-  <si>
-    <t>מלחייה</t>
-  </si>
-  <si>
-    <t>איחסון</t>
-  </si>
-  <si>
-    <t>פמוט</t>
-  </si>
-  <si>
     <t>נדרש תמונה</t>
   </si>
   <si>
-    <t>צלחת הגשה</t>
-  </si>
-  <si>
-    <t>סט קפה</t>
-  </si>
-  <si>
-    <t>מגש גבינות</t>
-  </si>
-  <si>
     <t>כלי עבודה</t>
   </si>
   <si>
-    <t>מטחנה</t>
-  </si>
-  <si>
-    <t>סל</t>
-  </si>
-  <si>
-    <t>פומפיה</t>
-  </si>
-  <si>
     <t>תבנית עוגה מקסימה</t>
   </si>
   <si>
-    <t>תבנית</t>
-  </si>
-  <si>
     <t>תבנית עוגה קטנה</t>
   </si>
   <si>
@@ -382,18 +337,12 @@
     <t>סל ביצים פתוח, חוט מתכת</t>
   </si>
   <si>
-    <t>הגשה</t>
-  </si>
-  <si>
     <t>ארון שתי דלתות</t>
   </si>
   <si>
     <t>ריהוט</t>
   </si>
   <si>
-    <t>ארון</t>
-  </si>
-  <si>
     <t>ארון מטבח שני חלקים</t>
   </si>
   <si>
@@ -406,9 +355,6 @@
     <t>שידת מגירות</t>
   </si>
   <si>
-    <t>שידה</t>
-  </si>
-  <si>
     <t>ארון ויטרינה</t>
   </si>
   <si>
@@ -430,28 +376,55 @@
     <t>שולחן כתיבה</t>
   </si>
   <si>
-    <t>שולחן</t>
-  </si>
-  <si>
     <t>ארונית תליה קטנה</t>
   </si>
   <si>
     <t>מדף צלחות</t>
   </si>
   <si>
-    <t>מדף</t>
-  </si>
-  <si>
     <t>מתלה לכלי מטבח</t>
   </si>
   <si>
-    <t>מתלה</t>
-  </si>
-  <si>
     <t>מדף אפור עם מתלים</t>
   </si>
   <si>
     <t>מדף לבן שתי קומות</t>
+  </si>
+  <si>
+    <t>כלי קיבול</t>
+  </si>
+  <si>
+    <t>כלי הגשה</t>
+  </si>
+  <si>
+    <t>פמוטים</t>
+  </si>
+  <si>
+    <t>כלי איחסון</t>
+  </si>
+  <si>
+    <t>כלי אחסון</t>
+  </si>
+  <si>
+    <t>תבניות</t>
+  </si>
+  <si>
+    <t>ארונות</t>
+  </si>
+  <si>
+    <t>שידות</t>
+  </si>
+  <si>
+    <t>שולחנות</t>
+  </si>
+  <si>
+    <t>מדפים</t>
+  </si>
+  <si>
+    <t>מתלים</t>
+  </si>
+  <si>
+    <t>ויטרינות</t>
   </si>
 </sst>
 </file>
@@ -792,8 +765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2417CC-E9D4-4575-BBAA-5E76F42A36C1}">
   <dimension ref="A2:L85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -838,7 +811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -852,7 +825,7 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="G3" s="1">
         <v>26.5</v>
@@ -873,7 +846,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -887,7 +860,7 @@
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G4" s="1">
         <v>28</v>
@@ -908,7 +881,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="98" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -922,7 +895,7 @@
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G5" s="1">
         <v>15.5</v>
@@ -943,7 +916,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -957,7 +930,7 @@
         <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="G6" s="1">
         <v>22</v>
@@ -978,7 +951,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="98" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -992,7 +965,7 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G7" s="1">
         <v>26</v>
@@ -1013,7 +986,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1027,7 +1000,7 @@
         <v>97</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="G8" s="1">
         <v>0</v>
@@ -1048,7 +1021,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="112" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="70" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -1062,7 +1035,7 @@
         <v>11</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G9" s="1">
         <v>19</v>
@@ -1083,7 +1056,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -1097,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G10" s="1">
         <v>26</v>
@@ -1118,9 +1091,9 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
@@ -1135,7 +1108,7 @@
         <v>11</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="G11" s="1">
         <v>38.5</v>
@@ -1156,7 +1129,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="84" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -1170,7 +1143,7 @@
         <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="G12" s="1">
         <v>16.5</v>
@@ -1191,7 +1164,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -1205,7 +1178,7 @@
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G13" s="1">
         <v>21</v>
@@ -1226,7 +1199,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="98" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -1240,7 +1213,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G14" s="1">
         <v>25</v>
@@ -1261,7 +1234,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -1275,7 +1248,7 @@
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1296,7 +1269,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -1310,7 +1283,7 @@
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -1331,7 +1304,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -1345,7 +1318,7 @@
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -1366,7 +1339,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -1380,7 +1353,7 @@
         <v>11</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G18" s="1">
         <v>13.5</v>
@@ -1401,7 +1374,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -1415,7 +1388,7 @@
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G19" s="1">
         <v>7.5</v>
@@ -1450,7 +1423,7 @@
         <v>11</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1471,7 +1444,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="84" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -1485,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -1506,7 +1479,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -1520,7 +1493,7 @@
         <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G22" s="1">
         <v>0</v>
@@ -1541,7 +1514,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -1555,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G23" s="1">
         <v>0</v>
@@ -1576,7 +1549,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="42" x14ac:dyDescent="0.3">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -1590,7 +1563,7 @@
         <v>11</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="G24" s="1">
         <v>0</v>
@@ -1611,7 +1584,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="112" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -1625,7 +1598,7 @@
         <v>11</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="G25" s="1">
         <v>0</v>
@@ -1646,7 +1619,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -1660,7 +1633,7 @@
         <v>11</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="G26" s="1">
         <v>20.5</v>
@@ -1681,7 +1654,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -1695,7 +1668,7 @@
         <v>11</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="G27" s="1">
         <v>15</v>
@@ -1716,7 +1689,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B28" s="1">
         <v>26</v>
       </c>
@@ -1730,7 +1703,7 @@
         <v>11</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G28" s="1">
         <v>33</v>
@@ -1751,7 +1724,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B29" s="1">
         <v>27</v>
       </c>
@@ -1765,7 +1738,7 @@
         <v>11</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G29" s="1">
         <v>36.5</v>
@@ -1786,7 +1759,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B30" s="1">
         <v>28</v>
       </c>
@@ -1800,7 +1773,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G30" s="1">
         <v>42.5</v>
@@ -1821,7 +1794,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
         <v>29</v>
       </c>
@@ -1835,7 +1808,7 @@
         <v>11</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G31" s="1">
         <v>40</v>
@@ -1856,7 +1829,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B32" s="1">
         <v>30</v>
       </c>
@@ -1870,7 +1843,7 @@
         <v>11</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G32" s="1">
         <v>44.5</v>
@@ -1891,7 +1864,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="33" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B33" s="1">
         <v>31</v>
       </c>
@@ -1905,7 +1878,7 @@
         <v>11</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G33" s="1">
         <v>33.5</v>
@@ -1926,7 +1899,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="34" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="1">
         <v>32</v>
       </c>
@@ -1940,7 +1913,7 @@
         <v>11</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G34" s="1">
         <v>25</v>
@@ -1961,7 +1934,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="35" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="1">
         <v>33</v>
       </c>
@@ -1975,7 +1948,7 @@
         <v>11</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G35" s="1">
         <v>12</v>
@@ -1996,7 +1969,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="1">
         <v>34</v>
       </c>
@@ -2010,7 +1983,7 @@
         <v>11</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G36" s="1">
         <v>10</v>
@@ -2031,7 +2004,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="37" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="1">
         <v>35</v>
       </c>
@@ -2045,7 +2018,7 @@
         <v>97</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="G37" s="1">
         <v>21</v>
@@ -2066,7 +2039,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="38" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="1">
         <v>36</v>
       </c>
@@ -2080,7 +2053,7 @@
         <v>11</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="G38" s="1">
         <v>14</v>
@@ -2101,7 +2074,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="1">
         <v>37</v>
       </c>
@@ -2112,10 +2085,10 @@
         <v>47</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>98</v>
+        <v>126</v>
       </c>
       <c r="G39" s="1">
         <v>11.5</v>
@@ -2136,7 +2109,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="1">
         <v>38</v>
       </c>
@@ -2150,7 +2123,7 @@
         <v>97</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G40" s="1">
         <v>12</v>
@@ -2171,7 +2144,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B41" s="1">
         <v>39</v>
       </c>
@@ -2185,7 +2158,7 @@
         <v>11</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G41" s="1">
         <v>20</v>
@@ -2206,7 +2179,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="42" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B42" s="1">
         <v>40</v>
       </c>
@@ -2220,7 +2193,7 @@
         <v>11</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G42" s="1">
         <v>25</v>
@@ -2241,7 +2214,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="43" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B43" s="1">
         <v>41</v>
       </c>
@@ -2255,7 +2228,7 @@
         <v>11</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G43" s="1">
         <v>16.5</v>
@@ -2276,7 +2249,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="44" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B44" s="1">
         <v>42</v>
       </c>
@@ -2290,7 +2263,7 @@
         <v>11</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="G44" s="1">
         <v>8</v>
@@ -2311,7 +2284,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="45" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B45" s="1">
         <v>43</v>
       </c>
@@ -2325,7 +2298,7 @@
         <v>97</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="G45" s="1">
         <v>37.5</v>
@@ -2360,7 +2333,7 @@
         <v>97</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="G46" s="1">
         <v>24.5</v>
@@ -2381,7 +2354,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B47" s="1">
         <v>45</v>
       </c>
@@ -2395,7 +2368,7 @@
         <v>97</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G47" s="1">
         <v>13.5</v>
@@ -2416,7 +2389,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B48" s="1">
         <v>46</v>
       </c>
@@ -2430,7 +2403,7 @@
         <v>11</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -2451,7 +2424,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B49" s="1">
         <v>47</v>
       </c>
@@ -2465,7 +2438,7 @@
         <v>11</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G49" s="1">
         <v>23</v>
@@ -2486,7 +2459,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="50" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>48</v>
       </c>
@@ -2500,7 +2473,7 @@
         <v>11</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G50" s="1">
         <v>23</v>
@@ -2521,7 +2494,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="51" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B51" s="1">
         <v>49</v>
       </c>
@@ -2535,7 +2508,7 @@
         <v>11</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G51" s="1">
         <v>22</v>
@@ -2556,7 +2529,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="52" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B52" s="1">
         <v>50</v>
       </c>
@@ -2570,7 +2543,7 @@
         <v>11</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="G52" s="1">
         <v>48</v>
@@ -2591,7 +2564,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="53" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B53" s="1">
         <v>51</v>
       </c>
@@ -2605,7 +2578,7 @@
         <v>11</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G53" s="1">
         <v>13</v>
@@ -2626,12 +2599,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="54" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B54" s="1">
         <v>52</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>70</v>
@@ -2640,7 +2613,7 @@
         <v>11</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G54" s="1">
         <v>12</v>
@@ -2661,7 +2634,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B55" s="1">
         <v>53</v>
       </c>
@@ -2675,7 +2648,7 @@
         <v>11</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G55" s="1">
         <v>12</v>
@@ -2696,12 +2669,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="56" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B56" s="1">
         <v>54</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>70</v>
@@ -2710,7 +2683,7 @@
         <v>11</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G56" s="1">
         <v>8</v>
@@ -2731,7 +2704,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="57" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B57" s="1">
         <v>55</v>
       </c>
@@ -2745,7 +2718,7 @@
         <v>11</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G57" s="1">
         <v>7</v>
@@ -2766,12 +2739,12 @@
         <v>250</v>
       </c>
     </row>
-    <row r="58" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B58" s="1">
         <v>56</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>70</v>
@@ -2780,7 +2753,7 @@
         <v>11</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
@@ -2801,7 +2774,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B59" s="1">
         <v>57</v>
       </c>
@@ -2815,7 +2788,7 @@
         <v>11</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G59" s="1">
         <v>0</v>
@@ -2836,7 +2809,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="60" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B60" s="1">
         <v>58</v>
       </c>
@@ -2850,7 +2823,7 @@
         <v>11</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="G60" s="1">
         <v>0</v>
@@ -2871,7 +2844,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="61" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B61" s="1">
         <v>59</v>
       </c>
@@ -2885,7 +2858,7 @@
         <v>11</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G61" s="1">
         <v>27</v>
@@ -2906,12 +2879,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="62" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B62" s="1">
         <v>60</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>70</v>
@@ -2920,7 +2893,7 @@
         <v>11</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G62" s="1">
         <v>23</v>
@@ -2941,7 +2914,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="63" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B63" s="1">
         <v>61</v>
       </c>
@@ -2955,7 +2928,7 @@
         <v>11</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G63" s="1">
         <v>21.5</v>
@@ -2976,7 +2949,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="64" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B64" s="1">
         <v>62</v>
       </c>
@@ -2990,7 +2963,7 @@
         <v>11</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G64" s="1">
         <v>24</v>
@@ -3011,7 +2984,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="65" spans="2:12" ht="28" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B65" s="1">
         <v>63</v>
       </c>
@@ -3025,7 +2998,7 @@
         <v>97</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G65" s="1">
         <v>20.5</v>
@@ -3046,7 +3019,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="66" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B66" s="1">
         <v>64</v>
       </c>
@@ -3060,7 +3033,7 @@
         <v>97</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G66" s="1">
         <v>25</v>
@@ -3081,7 +3054,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="67" spans="2:12" ht="42" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B67" s="1">
         <v>65</v>
       </c>
@@ -3095,7 +3068,7 @@
         <v>97</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G67" s="1">
         <v>10</v>
@@ -3116,7 +3089,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="68" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B68" s="1">
         <v>66</v>
       </c>
@@ -3130,7 +3103,7 @@
         <v>97</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>99</v>
+        <v>124</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -3151,7 +3124,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="69" spans="2:12" ht="56" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B69" s="1">
         <v>67</v>
       </c>
@@ -3165,7 +3138,7 @@
         <v>97</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="G69" s="1">
         <v>14.5</v>
@@ -3186,7 +3159,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="70" spans="2:12" ht="70" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:12" ht="28" x14ac:dyDescent="0.3">
       <c r="B70" s="1">
         <v>68</v>
       </c>
@@ -3197,10 +3170,10 @@
         <v>95</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="G70" s="1">
         <v>30</v>
@@ -3226,16 +3199,16 @@
         <v>69</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G71" s="1">
         <v>122</v>
@@ -3250,7 +3223,7 @@
         <v>0</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="L71" s="1">
         <v>3500</v>
@@ -3261,16 +3234,16 @@
         <v>70</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G72" s="1">
         <v>194</v>
@@ -3285,7 +3258,7 @@
         <v>0</v>
       </c>
       <c r="K72" s="1" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="L72" s="1">
         <v>5200</v>
@@ -3296,16 +3269,16 @@
         <v>71</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G73" s="1">
         <v>88</v>
@@ -3320,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="L73" s="1">
         <v>3500</v>
@@ -3331,16 +3304,16 @@
         <v>72</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G74" s="1">
         <v>93.5</v>
@@ -3355,7 +3328,7 @@
         <v>0</v>
       </c>
       <c r="K74" s="1" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="L74" s="1">
         <v>2800</v>
@@ -3366,16 +3339,16 @@
         <v>73</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="G75" s="1">
         <v>170</v>
@@ -3390,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="L75" s="1">
         <v>3800</v>
@@ -3401,16 +3374,16 @@
         <v>74</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G76" s="1">
         <v>78.5</v>
@@ -3425,7 +3398,7 @@
         <v>0</v>
       </c>
       <c r="K76" s="1" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="L76" s="1">
         <v>950</v>
@@ -3436,16 +3409,16 @@
         <v>75</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="G77" s="1">
         <v>114</v>
@@ -3460,7 +3433,7 @@
         <v>0</v>
       </c>
       <c r="K77" s="1" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="L77" s="1">
         <v>2800</v>
@@ -3471,16 +3444,16 @@
         <v>76</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G78" s="1">
         <v>95</v>
@@ -3495,7 +3468,7 @@
         <v>0</v>
       </c>
       <c r="K78" s="1" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="L78" s="1">
         <v>2950</v>
@@ -3506,16 +3479,16 @@
         <v>77</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G79" s="1">
         <v>97</v>
@@ -3530,7 +3503,7 @@
         <v>0</v>
       </c>
       <c r="K79" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="L79" s="1">
         <v>1700</v>
@@ -3541,16 +3514,16 @@
         <v>78</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="G80" s="1">
         <v>78</v>
@@ -3565,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="L80" s="1">
         <v>4500</v>
@@ -3576,16 +3549,16 @@
         <v>79</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G81" s="1">
         <v>60</v>
@@ -3600,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="L81" s="1">
         <v>800</v>
@@ -3611,16 +3584,16 @@
         <v>80</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G82" s="1">
         <v>73</v>
@@ -3635,7 +3608,7 @@
         <v>0</v>
       </c>
       <c r="K82" s="1" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="L82" s="1">
         <v>1200</v>
@@ -3646,16 +3619,16 @@
         <v>81</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="G83" s="1">
         <v>83</v>
@@ -3670,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="K83" s="1" t="s">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="L83" s="1">
         <v>1250</v>
@@ -3681,16 +3654,16 @@
         <v>82</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G84" s="1">
         <v>36</v>
@@ -3705,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="K84" s="1" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="L84" s="1">
         <v>850</v>
@@ -3716,16 +3689,16 @@
         <v>83</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="G85" s="1">
         <v>59</v>
@@ -3740,7 +3713,7 @@
         <v>0</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="L85" s="1">
         <v>1200</v>

</xml_diff>